<commit_message>
changed format of arrangements and practice arrangements
</commit_message>
<xml_diff>
--- a/docs/miscellaneous/choosing_arrangements.xlsx
+++ b/docs/miscellaneous/choosing_arrangements.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535E0EB6-DA3C-4CC9-9C52-0F21EAE3634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +14,9 @@
     <definedName name="Slicer_hidden_type">#N/A</definedName>
     <definedName name="Slicer_pa_type">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="20">
   <si>
     <t>arrangement</t>
   </si>
@@ -85,9 +84,6 @@
     <t>summed_min_row_col_dist</t>
   </si>
   <si>
-    <t>(blank)</t>
-  </si>
-  <si>
     <t>Count of arrangement</t>
   </si>
   <si>
@@ -105,12 +101,18 @@
   <si>
     <t>far-comp</t>
   </si>
+  <si>
+    <t>far</t>
+  </si>
+  <si>
+    <t>subtype</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +125,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -152,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -160,6 +168,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,8 +393,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -460,8 +471,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -534,7 +545,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Author" refreshedDate="44719.792092939817" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF22000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="44721.479857523147" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -595,7 +606,16 @@
       </sharedItems>
     </cacheField>
     <cacheField name="summed_min_row_col_dist" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="9"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="9" count="8">
+        <n v="3"/>
+        <n v="4"/>
+        <n v="8"/>
+        <n v="7"/>
+        <n v="5"/>
+        <n v="9"/>
+        <n v="2"/>
+        <n v="6"/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -607,7 +627,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="60">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -621,7 +641,7 @@
     <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -636,7 +656,7 @@
     <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -651,7 +671,7 @@
     <n v="5"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -666,7 +686,7 @@
     <n v="2"/>
     <n v="5"/>
     <x v="1"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
@@ -681,7 +701,7 @@
     <n v="4"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="0"/>
@@ -696,7 +716,7 @@
     <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -711,7 +731,7 @@
     <n v="5"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="0"/>
@@ -726,7 +746,7 @@
     <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -741,7 +761,7 @@
     <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -756,7 +776,7 @@
     <n v="5"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="0"/>
@@ -771,22 +791,22 @@
     <n v="4"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
     <n v="3"/>
-    <n v="10"/>
-    <n v="2"/>
     <n v="9"/>
+    <n v="2"/>
+    <n v="8"/>
     <n v="9"/>
-    <n v="2"/>
-    <n v="2"/>
-    <n v="2"/>
-    <x v="1"/>
-    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="1"/>
@@ -801,7 +821,7 @@
     <n v="3"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="1"/>
@@ -816,7 +836,7 @@
     <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -831,7 +851,7 @@
     <n v="1"/>
     <n v="4"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="1"/>
@@ -846,7 +866,7 @@
     <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
@@ -861,7 +881,7 @@
     <n v="5"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
@@ -876,7 +896,7 @@
     <n v="3"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="1"/>
@@ -891,7 +911,7 @@
     <n v="4"/>
     <n v="5"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="1"/>
@@ -906,7 +926,7 @@
     <n v="5"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
@@ -921,7 +941,7 @@
     <n v="5"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
@@ -936,7 +956,7 @@
     <n v="4"/>
     <n v="5"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="1"/>
@@ -951,7 +971,7 @@
     <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="1"/>
@@ -966,7 +986,7 @@
     <n v="1"/>
     <n v="4"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="2"/>
@@ -981,7 +1001,7 @@
     <n v="2"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -996,7 +1016,7 @@
     <n v="5"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="2"/>
@@ -1011,7 +1031,7 @@
     <n v="1"/>
     <n v="4"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="2"/>
@@ -1026,7 +1046,7 @@
     <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="2"/>
@@ -1041,7 +1061,7 @@
     <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -1056,7 +1076,7 @@
     <n v="2"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -1071,7 +1091,7 @@
     <n v="5"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="2"/>
@@ -1086,7 +1106,7 @@
     <n v="4"/>
     <n v="5"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="2"/>
@@ -1101,7 +1121,7 @@
     <n v="4"/>
     <n v="5"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="2"/>
@@ -1116,7 +1136,7 @@
     <n v="5"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="2"/>
@@ -1131,7 +1151,7 @@
     <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="2"/>
@@ -1146,7 +1166,7 @@
     <n v="1"/>
     <n v="4"/>
     <x v="0"/>
-    <n v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="3"/>
@@ -1161,7 +1181,7 @@
     <n v="1"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="2"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="3"/>
@@ -1176,7 +1196,7 @@
     <n v="3"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="3"/>
@@ -1191,7 +1211,7 @@
     <n v="2"/>
     <n v="5"/>
     <x v="1"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="3"/>
@@ -1206,7 +1226,7 @@
     <n v="4"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="3"/>
@@ -1221,7 +1241,7 @@
     <n v="5"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="3"/>
@@ -1236,7 +1256,7 @@
     <n v="2"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -1251,7 +1271,7 @@
     <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="3"/>
@@ -1266,7 +1286,7 @@
     <n v="4"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="3"/>
@@ -1281,7 +1301,7 @@
     <n v="4"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="3"/>
@@ -1296,7 +1316,7 @@
     <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="3"/>
@@ -1311,7 +1331,7 @@
     <n v="1"/>
     <n v="3"/>
     <x v="0"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="3"/>
@@ -1326,7 +1346,7 @@
     <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="4"/>
@@ -1341,7 +1361,7 @@
     <n v="2"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -1356,7 +1376,7 @@
     <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -1371,7 +1391,7 @@
     <n v="2"/>
     <n v="5"/>
     <x v="1"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
@@ -1386,7 +1406,7 @@
     <n v="5"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="4"/>
@@ -1401,7 +1421,7 @@
     <n v="4"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="4"/>
@@ -1416,7 +1436,7 @@
     <n v="1"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="2"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="4"/>
@@ -1431,7 +1451,7 @@
     <n v="5"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="4"/>
@@ -1446,7 +1466,7 @@
     <n v="4"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
@@ -1461,7 +1481,7 @@
     <n v="4"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
@@ -1476,7 +1496,7 @@
     <n v="5"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="9"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="4"/>
@@ -1491,29 +1511,29 @@
     <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="4"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
     <n v="11"/>
-    <n v="8"/>
+    <n v="7"/>
     <n v="10"/>
-    <n v="7"/>
+    <n v="6"/>
     <n v="1"/>
-    <n v="4"/>
+    <n v="5"/>
     <n v="1"/>
-    <n v="4"/>
-    <x v="0"/>
-    <n v="5"/>
+    <n v="5"/>
+    <x v="0"/>
+    <x v="7"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A1:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A1:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="13">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="5">
@@ -1531,8 +1551,8 @@
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="2">
-        <item h="1" x="1"/>
-        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -1543,7 +1563,7 @@
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="3">
         <item x="1"/>
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item x="2"/>
       </items>
       <extLst>
@@ -1608,7 +1628,7 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="5">
         <item x="0"/>
         <item x="1"/>
@@ -1622,7 +1642,17 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="6"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="5"/>
+      </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
@@ -1635,10 +1665,26 @@
     <field x="2"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="10">
     <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
       <x v="1"/>
-      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
       <x/>
     </i>
     <i r="2">
@@ -1655,17 +1701,17 @@
     </i>
   </rowItems>
   <colFields count="1">
-    <field x="11"/>
+    <field x="12"/>
   </colFields>
   <colItems count="3">
     <i>
-      <x/>
+      <x v="5"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="6"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="7"/>
     </i>
   </colItems>
   <dataFields count="1">
@@ -1684,15 +1730,15 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_pa_type" xr10:uid="{00000000-0013-0000-FFFF-FFFF01000000}" sourceName="pa_type">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_pa_type" sourceName="pa_type">
   <pivotTables>
     <pivotTable tabId="2" name="PivotTable1"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
       <items count="2">
-        <i x="1"/>
-        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="0" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -1700,16 +1746,16 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_hidden_type" xr10:uid="{00000000-0013-0000-FFFF-FFFF02000000}" sourceName="hidden_type">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_hidden_type" sourceName="hidden_type">
   <pivotTables>
     <pivotTable tabId="2" name="PivotTable1"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
       <items count="3">
-        <i x="0" s="1"/>
-        <i x="2" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
+        <i x="2" s="1"/>
+        <i x="1" s="1"/>
+        <i x="0"/>
       </items>
     </tabular>
   </data>
@@ -1717,43 +1763,43 @@
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="pa_type" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="Slicer_pa_type" caption="pa_type" rowHeight="241300"/>
-  <slicer name="hidden_type" xr10:uid="{00000000-0014-0000-FFFF-FFFF02000000}" cache="Slicer_hidden_type" caption="hidden_type" rowHeight="241300"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="pa_type" cache="Slicer_pa_type" caption="pa_type" rowHeight="241300"/>
+  <slicer name="hidden_type" cache="Slicer_hidden_type" caption="hidden_type" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M61" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A1:M61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M79" totalsRowShown="0" dataDxfId="13">
+  <autoFilter ref="A1:M79"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="arrangement" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pa_type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="hidden_type" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="row" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="column" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="row_dist" dataDxfId="7">
+    <tableColumn id="1" name="arrangement" dataDxfId="12"/>
+    <tableColumn id="2" name="pa_type" dataDxfId="11"/>
+    <tableColumn id="3" name="subtype" dataDxfId="10"/>
+    <tableColumn id="4" name="row" dataDxfId="9"/>
+    <tableColumn id="5" name="column" dataDxfId="8"/>
+    <tableColumn id="6" name="row_dist" dataDxfId="7">
       <calculatedColumnFormula>D2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="col_dist" dataDxfId="6">
+    <tableColumn id="7" name="col_dist" dataDxfId="6">
       <calculatedColumnFormula>E2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="row_dist_other_way" dataDxfId="5">
+    <tableColumn id="8" name="row_dist_other_way" dataDxfId="5">
       <calculatedColumnFormula>12-D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="col_dist_other_way" dataDxfId="4">
+    <tableColumn id="9" name="col_dist_other_way" dataDxfId="4">
       <calculatedColumnFormula>12-E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="min_row_dist" dataDxfId="3">
+    <tableColumn id="10" name="min_row_dist" dataDxfId="3">
       <calculatedColumnFormula>MIN(F2,H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="min_col_dist" dataDxfId="2">
+    <tableColumn id="11" name="min_col_dist" dataDxfId="2">
       <calculatedColumnFormula>MIN(G2,I2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="min_row_col_dist" dataDxfId="1">
+    <tableColumn id="12" name="min_row_col_dist" dataDxfId="1">
       <calculatedColumnFormula>MIN(J2:K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="summed_min_row_col_dist" dataDxfId="0">
+    <tableColumn id="13" name="summed_min_row_col_dist" dataDxfId="0">
       <calculatedColumnFormula>J2+K2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2023,32 +2069,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="28.5546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="4" customWidth="1"/>
     <col min="11" max="11" width="20" style="4" customWidth="1"/>
-    <col min="12" max="12" width="26.109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="36.88671875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="4"/>
+    <col min="12" max="12" width="26.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="36.85546875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -2065,16 +2111,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -2089,7 +2135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2136,7 +2182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2183,14 +2229,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="5">
         <v>7</v>
       </c>
@@ -2230,14 +2278,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="5">
         <v>3</v>
       </c>
@@ -2277,7 +2327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -2324,7 +2374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -2371,7 +2421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -2420,7 +2470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -2469,7 +2519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -2518,7 +2568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -2567,7 +2617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1</v>
       </c>
@@ -2614,7 +2664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
@@ -2626,7 +2676,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
@@ -2634,7 +2684,7 @@
       </c>
       <c r="G13" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="2"/>
@@ -2642,7 +2692,7 @@
       </c>
       <c r="I13" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="4"/>
@@ -2650,7 +2700,7 @@
       </c>
       <c r="K13" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="6"/>
@@ -2658,10 +2708,10 @@
       </c>
       <c r="M13" s="5">
         <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2</v>
       </c>
@@ -2708,7 +2758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2755,7 +2805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -2802,14 +2852,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D17" s="5">
         <v>9</v>
       </c>
@@ -2849,14 +2901,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D18" s="5">
         <v>7</v>
       </c>
@@ -2896,7 +2950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2</v>
       </c>
@@ -2943,7 +2997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>2</v>
       </c>
@@ -2992,7 +3046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -3041,7 +3095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>2</v>
       </c>
@@ -3090,7 +3144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2</v>
       </c>
@@ -3139,7 +3193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2</v>
       </c>
@@ -3186,7 +3240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>2</v>
       </c>
@@ -3233,7 +3287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>3</v>
       </c>
@@ -3280,14 +3334,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D27" s="5">
         <v>7</v>
       </c>
@@ -3327,7 +3383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>3</v>
       </c>
@@ -3374,14 +3430,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D29" s="5">
         <v>4</v>
       </c>
@@ -3421,7 +3479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>3</v>
       </c>
@@ -3468,7 +3526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>3</v>
       </c>
@@ -3515,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>3</v>
       </c>
@@ -3564,7 +3622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>3</v>
       </c>
@@ -3613,7 +3671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>3</v>
       </c>
@@ -3662,7 +3720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>3</v>
       </c>
@@ -3711,7 +3769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>3</v>
       </c>
@@ -3758,7 +3816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>3</v>
       </c>
@@ -3805,7 +3863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>4</v>
       </c>
@@ -3852,7 +3910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>4</v>
       </c>
@@ -3899,14 +3957,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>4</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D40" s="5">
         <v>10</v>
       </c>
@@ -3946,14 +4006,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>4</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D41" s="5">
         <v>8</v>
       </c>
@@ -3993,7 +4055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>4</v>
       </c>
@@ -4040,7 +4102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>4</v>
       </c>
@@ -4087,7 +4149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>4</v>
       </c>
@@ -4136,7 +4198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>4</v>
       </c>
@@ -4185,7 +4247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>4</v>
       </c>
@@ -4234,7 +4296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>4</v>
       </c>
@@ -4283,7 +4345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>4</v>
       </c>
@@ -4330,7 +4392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>4</v>
       </c>
@@ -4377,7 +4439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>5</v>
       </c>
@@ -4424,7 +4486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>5</v>
       </c>
@@ -4471,7 +4533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>5</v>
       </c>
@@ -4518,14 +4580,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>5</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D53" s="5">
         <v>7</v>
       </c>
@@ -4565,14 +4629,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>5</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D54" s="5">
         <v>5</v>
       </c>
@@ -4612,7 +4678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>5</v>
       </c>
@@ -4659,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>5</v>
       </c>
@@ -4708,7 +4774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>5</v>
       </c>
@@ -4757,7 +4823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>5</v>
       </c>
@@ -4806,7 +4872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>5</v>
       </c>
@@ -4855,7 +4921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>5</v>
       </c>
@@ -4902,7 +4968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>5</v>
       </c>
@@ -4914,7 +4980,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F61" s="6">
         <f t="shared" si="0"/>
@@ -4922,7 +4988,7 @@
       </c>
       <c r="G61" s="6">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H61" s="5">
         <f t="shared" si="2"/>
@@ -4930,7 +4996,7 @@
       </c>
       <c r="I61" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J61" s="5">
         <f t="shared" si="4"/>
@@ -4938,7 +5004,7 @@
       </c>
       <c r="K61" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L61" s="5">
         <f t="shared" si="6"/>
@@ -4946,6 +5012,864 @@
       </c>
       <c r="M61" s="5">
         <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>6</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7">
+        <v>5</v>
+      </c>
+      <c r="E62" s="7">
+        <v>2</v>
+      </c>
+      <c r="F62" s="8">
+        <f t="shared" ref="F62:F79" si="8">D62-1</f>
+        <v>4</v>
+      </c>
+      <c r="G62" s="8">
+        <f t="shared" ref="G62:G79" si="9">E62-1</f>
+        <v>1</v>
+      </c>
+      <c r="H62" s="9">
+        <f t="shared" ref="H62:H79" si="10">12-D62</f>
+        <v>7</v>
+      </c>
+      <c r="I62" s="9">
+        <f t="shared" ref="I62:I79" si="11">12-E62</f>
+        <v>10</v>
+      </c>
+      <c r="J62" s="9">
+        <f t="shared" ref="J62:J79" si="12">MIN(F62,H62)</f>
+        <v>4</v>
+      </c>
+      <c r="K62" s="9">
+        <f t="shared" ref="K62:K79" si="13">MIN(G62,I62)</f>
+        <v>1</v>
+      </c>
+      <c r="L62" s="9">
+        <f t="shared" ref="L62:L79" si="14">MIN(J62:K62)</f>
+        <v>1</v>
+      </c>
+      <c r="M62" s="9">
+        <f t="shared" ref="M62:M79" si="15">J62+K62</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>6</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7">
+        <v>10</v>
+      </c>
+      <c r="E63" s="7">
+        <v>5</v>
+      </c>
+      <c r="F63" s="8">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="G63" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="H63" s="9">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="I63" s="9">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="J63" s="9">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K63" s="9">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="L63" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M63" s="9">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>6</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7">
+        <v>7</v>
+      </c>
+      <c r="E64" s="7">
+        <v>6</v>
+      </c>
+      <c r="F64" s="8">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="G64" s="8">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="H64" s="9">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="I64" s="9">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="J64" s="9">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="K64" s="9">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="L64" s="9">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="M64" s="9">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>6</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7">
+        <v>3</v>
+      </c>
+      <c r="E65" s="7">
+        <v>8</v>
+      </c>
+      <c r="F65" s="8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G65" s="8">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="H65" s="9">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="I65" s="9">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="J65" s="9">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K65" s="9">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="L65" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M65" s="9">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>6</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7">
+        <v>11</v>
+      </c>
+      <c r="E66" s="7">
+        <v>10</v>
+      </c>
+      <c r="F66" s="8">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="G66" s="8">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="H66" s="9">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I66" s="9">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="J66" s="9">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K66" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L66" s="9">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M66" s="9">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>6</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="7">
+        <v>4</v>
+      </c>
+      <c r="E67" s="7">
+        <v>11</v>
+      </c>
+      <c r="F67" s="8">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G67" s="8">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="H67" s="9">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="I67" s="9">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="J67" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K67" s="9">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="L67" s="9">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M67" s="9">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <v>6</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7">
+        <v>9</v>
+      </c>
+      <c r="E68" s="7">
+        <v>3</v>
+      </c>
+      <c r="F68" s="8">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G68" s="8">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="H68" s="9">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="I68" s="9">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="J68" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K68" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L68" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M68" s="9">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
+        <v>6</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7">
+        <v>2</v>
+      </c>
+      <c r="E69" s="7">
+        <v>5</v>
+      </c>
+      <c r="F69" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G69" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="H69" s="9">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I69" s="9">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="J69" s="9">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K69" s="9">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="L69" s="9">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M69" s="9">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>6</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="7">
+        <v>4</v>
+      </c>
+      <c r="E70" s="7">
+        <v>10</v>
+      </c>
+      <c r="F70" s="8">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G70" s="8">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="H70" s="9">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="I70" s="9">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="J70" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K70" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L70" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M70" s="9">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>7</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7">
+        <v>4</v>
+      </c>
+      <c r="E71" s="7">
+        <v>2</v>
+      </c>
+      <c r="F71" s="8">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G71" s="8">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H71" s="9">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="I71" s="9">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="J71" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K71" s="9">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="L71" s="9">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M71" s="9">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>7</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7">
+        <v>11</v>
+      </c>
+      <c r="E72" s="7">
+        <v>3</v>
+      </c>
+      <c r="F72" s="8">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="G72" s="8">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="H72" s="9">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I72" s="9">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="J72" s="9">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K72" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L72" s="9">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M72" s="9">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>7</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7">
+        <v>9</v>
+      </c>
+      <c r="E73" s="7">
+        <v>6</v>
+      </c>
+      <c r="F73" s="8">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G73" s="8">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="H73" s="9">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="I73" s="9">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="J73" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K73" s="9">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="L73" s="9">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="M73" s="9">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>7</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="7">
+        <v>5</v>
+      </c>
+      <c r="E74" s="7">
+        <v>7</v>
+      </c>
+      <c r="F74" s="8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="G74" s="8">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="H74" s="9">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="I74" s="9">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="J74" s="9">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="K74" s="9">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="L74" s="9">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M74" s="9">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>7</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7">
+        <v>3</v>
+      </c>
+      <c r="E75" s="7">
+        <v>8</v>
+      </c>
+      <c r="F75" s="8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G75" s="8">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="H75" s="9">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="I75" s="9">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="J75" s="9">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K75" s="9">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="L75" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M75" s="9">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
+        <v>7</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="7">
+        <v>8</v>
+      </c>
+      <c r="E76" s="7">
+        <v>10</v>
+      </c>
+      <c r="F76" s="8">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="G76" s="8">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="H76" s="9">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="I76" s="9">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="J76" s="9">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="K76" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L76" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M76" s="9">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>7</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7">
+        <v>8</v>
+      </c>
+      <c r="E77" s="7">
+        <v>3</v>
+      </c>
+      <c r="F77" s="8">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="G77" s="8">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="H77" s="9">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="I77" s="9">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="J77" s="9">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="K77" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L77" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M77" s="9">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>7</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="7">
+        <v>5</v>
+      </c>
+      <c r="E78" s="7">
+        <v>6</v>
+      </c>
+      <c r="F78" s="8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="G78" s="8">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="H78" s="9">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="I78" s="9">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="J78" s="9">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="K78" s="9">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="L78" s="9">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M78" s="9">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>7</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="7">
+        <v>9</v>
+      </c>
+      <c r="E79" s="7">
+        <v>10</v>
+      </c>
+      <c r="F79" s="8">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G79" s="8">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="H79" s="9">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="I79" s="9">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="J79" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K79" s="9">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L79" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M79" s="9">
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
     </row>
@@ -4959,31 +5883,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="2" customWidth="1"/>
+    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4994,48 +5919,44 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2">
         <v>1</v>
       </c>
@@ -5043,19 +5964,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2">
         <v>1</v>
       </c>
@@ -5063,43 +5982,125 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
-        <v>4</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>